<commit_message>
Added USB section to documentation. Adjusted schedule slightly due to my delay from traveling.
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Potential cause(s)</t>
   </si>
   <si>
-    <t>mission phase</t>
-  </si>
-  <si>
     <t>local effects of failure</t>
   </si>
   <si>
@@ -175,6 +172,15 @@
   </si>
   <si>
     <t>FMEA Ref. #</t>
+  </si>
+  <si>
+    <t>Manual Remote Board</t>
+  </si>
+  <si>
+    <t>Drive enable switch</t>
+  </si>
+  <si>
+    <t>Mode Selector</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -261,6 +267,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,55 +308,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -368,6 +329,61 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -389,6 +405,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -410,30 +443,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -449,14 +458,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:P20" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="B4:P20"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B5:O21" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="B5:O21"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="FMEA Ref. #"/>
     <tableColumn id="2" name="Item"/>
     <tableColumn id="3" name="Potential failure mode"/>
     <tableColumn id="4" name="Potential cause(s)"/>
-    <tableColumn id="5" name="mission phase"/>
     <tableColumn id="6" name="local effects of failure"/>
     <tableColumn id="7" name="next higher level effect"/>
     <tableColumn id="8" name="system level end effect"/>
@@ -473,40 +481,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:C9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="11"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="12"/>
+    <tableColumn id="1" name="Rating" dataDxfId="18"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="B13:C19"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="9"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="10"/>
+    <tableColumn id="1" name="Rating" dataDxfId="14"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="B23:C29"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="7"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="8"/>
+    <tableColumn id="1" name="Rating" dataDxfId="10"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="G4:M9"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Probability \ Severity" dataDxfId="6"/>
@@ -808,84 +816,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P27"/>
+  <dimension ref="B2:O28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="44.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="31.42578125" customWidth="1"/>
-    <col min="15" max="15" width="26.5703125" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="8" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="44.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="L5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="2:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="2:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -918,263 +952,263 @@
   <sheetData>
     <row r="3" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1182,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1190,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1198,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1206,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1214,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1222,7 +1256,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed FMEA of manual remote
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="132">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -48,9 +48,6 @@
     <t>(S) Severity</t>
   </si>
   <si>
-    <t>Detection (indications to Operator, Maintainer)</t>
-  </si>
-  <si>
     <t>Risk Level</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>Mitigation / Requirements</t>
   </si>
   <si>
-    <t>(D) Detection Dormancy Period</t>
-  </si>
-  <si>
-    <t>Risk Level  =P*S+D</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
@@ -379,13 +370,58 @@
   </si>
   <si>
     <t>JP9 (aux switch/ LEDs)</t>
+  </si>
+  <si>
+    <t>dielectric breakdown</t>
+  </si>
+  <si>
+    <t>power supply shorted out</t>
+  </si>
+  <si>
+    <t>plugged in backwards</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>human error</t>
+  </si>
+  <si>
+    <t>excessive power</t>
+  </si>
+  <si>
+    <t>LEDs not functioning properly</t>
+  </si>
+  <si>
+    <t>power and gnd shorted</t>
+  </si>
+  <si>
+    <t>improper connectivity</t>
+  </si>
+  <si>
+    <t>shorting power supplies together</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>use connector with tab</t>
+  </si>
+  <si>
+    <t>board wont function</t>
+  </si>
+  <si>
+    <t>manual mode will not work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +448,14 @@
       <b/>
       <sz val="36"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -468,12 +512,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="35">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -681,12 +725,6 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -702,21 +740,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B5:O41" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="B5:O41"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="34"/>
-    <tableColumn id="2" name="Item" dataDxfId="33"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="32"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="31"/>
-    <tableColumn id="6" name="local effects of failure" dataDxfId="30"/>
-    <tableColumn id="7" name="next higher level effect" dataDxfId="29"/>
-    <tableColumn id="8" name="system level end effect" dataDxfId="28"/>
-    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="27"/>
-    <tableColumn id="10" name="(S) Severity" dataDxfId="26"/>
-    <tableColumn id="11" name="Detection (indications to Operator, Maintainer)" dataDxfId="25"/>
-    <tableColumn id="15" name="(D) Detection Dormancy Period" dataDxfId="24"/>
-    <tableColumn id="12" name="Risk Level  =P*S+D" dataDxfId="23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B5:M41" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="B5:M41"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="32"/>
+    <tableColumn id="2" name="Item" dataDxfId="31"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="30"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="29"/>
+    <tableColumn id="6" name="local effects of failure" dataDxfId="28"/>
+    <tableColumn id="7" name="next higher level effect" dataDxfId="27"/>
+    <tableColumn id="8" name="system level end effect" dataDxfId="26"/>
+    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="25"/>
+    <tableColumn id="10" name="(S) Severity" dataDxfId="24"/>
+    <tableColumn id="12" name="Risk Level" dataDxfId="23"/>
     <tableColumn id="13" name="Actions for further Investigation" dataDxfId="22"/>
     <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="21"/>
   </tableColumns>
@@ -1060,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O47"/>
+  <dimension ref="B2:M47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,29 +1111,27 @@
     <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="25.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="44.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
@@ -1127,885 +1161,1319 @@
         <v>9</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F25" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <v>29</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-    </row>
-    <row r="35" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <v>30</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
         <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="47" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B47" s="5"/>
     </row>
   </sheetData>
@@ -2021,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,263 +2508,263 @@
   <sheetData>
     <row r="3" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="M9" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2304,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2312,7 +2780,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2320,7 +2788,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2328,7 +2796,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2336,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2344,7 +2812,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed stop mask on vias. Updated FMEA for R14.
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-14025" yWindow="855" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="-14025" yWindow="855" windowWidth="19440" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="FMEA" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">KEY!$A$1:$P$32</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="133">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -415,13 +415,16 @@
   </si>
   <si>
     <t>manual mode will not work</t>
+  </si>
+  <si>
+    <t>Use Active Pull-Down on GPIO (Recalculate external pull-down value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,22 +522,22 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -548,10 +551,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -569,10 +572,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -586,10 +589,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -607,10 +610,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -624,10 +627,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -645,10 +648,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -662,10 +665,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -683,49 +686,49 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -884,7 +887,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -919,7 +921,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1095,14 +1096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
@@ -1113,23 +1114,23 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" customWidth="1"/>
     <col min="12" max="12" width="26.5703125" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="2:13" ht="46.5">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:13" ht="46.5">
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" ht="28.5">
       <c r="B4" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="31.5" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13">
       <c r="B6" s="11">
         <v>1</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13">
       <c r="B7" s="11">
         <v>2</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13">
       <c r="B8" s="11">
         <v>3</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13">
       <c r="B9" s="11">
         <v>4</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13">
       <c r="B10" s="11">
         <v>5</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13">
       <c r="B11" s="11">
         <v>6</v>
       </c>
@@ -1375,7 +1376,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13">
       <c r="B12" s="11">
         <v>7</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13">
       <c r="B13" s="11">
         <v>8</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="30">
       <c r="B14" s="11">
         <v>9</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13">
       <c r="B15" s="11">
         <v>10</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13">
       <c r="B16" s="11">
         <v>11</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="30">
       <c r="B17" s="11">
         <v>12</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="30">
       <c r="B18" s="11">
         <v>13</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="75">
       <c r="B19" s="11">
         <v>14</v>
       </c>
@@ -1662,10 +1663,10 @@
         <v>121</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="30">
       <c r="B20" s="11">
         <v>15</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="30">
       <c r="B21" s="11">
         <v>16</v>
       </c>
@@ -1737,7 +1738,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="11">
         <v>17</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="B23" s="11">
         <v>18</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13">
       <c r="B24" s="11">
         <v>19</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13">
       <c r="B25" s="11">
         <v>20</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="15.75" customHeight="1">
       <c r="B26" s="11">
         <v>21</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="30">
       <c r="B27" s="11">
         <v>22</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="30">
       <c r="B28" s="11">
         <v>23</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="30">
       <c r="B29" s="11">
         <v>24</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" ht="30">
       <c r="B30" s="11">
         <v>25</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" ht="30">
       <c r="B31" s="11">
         <v>26</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="11">
         <v>27</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" ht="30">
       <c r="B33" s="11">
         <v>28</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13">
       <c r="B34" s="11">
         <v>29</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" ht="30">
       <c r="B35" s="11">
         <v>30</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13">
       <c r="B36" s="11">
         <v>31</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13">
       <c r="B37" s="11">
         <v>32</v>
       </c>
@@ -2321,7 +2322,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" ht="30">
       <c r="B38" s="11">
         <v>33</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" ht="30">
       <c r="B39" s="11">
         <v>34</v>
       </c>
@@ -2397,7 +2398,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" ht="30">
       <c r="B40" s="11">
         <v>35</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13">
       <c r="B41" s="11">
         <v>36</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="47" spans="2:13" ht="46.5">
       <c r="B47" s="5"/>
     </row>
   </sheetData>
@@ -2486,14 +2487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="58.5703125" customWidth="1"/>
@@ -2506,7 +2507,7 @@
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:13" ht="50.1" customHeight="1">
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
@@ -2515,7 +2516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" ht="50.1" customHeight="1">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="50.1" customHeight="1">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="50.1" customHeight="1">
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="50.1" customHeight="1">
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="50.1" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="50.1" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
@@ -2689,14 +2690,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:13" ht="50.1" customHeight="1"/>
+    <row r="11" spans="2:13" ht="50.1" customHeight="1"/>
+    <row r="12" spans="2:13" ht="50.1" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:13" ht="50.1" customHeight="1">
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="50.1" customHeight="1">
       <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="50.1" customHeight="1">
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="50.1" customHeight="1">
       <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +2729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="50.1" customHeight="1">
       <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="50.1" customHeight="1">
       <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="50.1" customHeight="1">
       <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2752,14 +2753,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:3" ht="50.1" customHeight="1"/>
+    <row r="21" spans="2:3" ht="50.1" customHeight="1"/>
+    <row r="22" spans="2:3" ht="50.1" customHeight="1">
       <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:3" ht="50.1" customHeight="1">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" ht="50.1" customHeight="1">
       <c r="B24" s="8">
         <v>1</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="50.1" customHeight="1">
       <c r="B25" s="7">
         <v>2</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" ht="50.1" customHeight="1">
       <c r="B26" s="7">
         <v>3</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" ht="50.1" customHeight="1">
       <c r="B27" s="7">
         <v>4</v>
       </c>
@@ -2799,7 +2800,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" ht="50.1" customHeight="1">
       <c r="B28" s="7">
         <v>5</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" ht="50.1" customHeight="1">
       <c r="B29" s="7">
         <v>6</v>
       </c>
@@ -2815,14 +2816,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:3" ht="50.1" customHeight="1"/>
+    <row r="31" spans="2:3" ht="50.1" customHeight="1"/>
+    <row r="32" spans="2:3" ht="50.1" customHeight="1"/>
+    <row r="33" ht="50.1" customHeight="1"/>
+    <row r="34" ht="50.1" customHeight="1"/>
+    <row r="35" ht="50.1" customHeight="1"/>
+    <row r="36" ht="50.1" customHeight="1"/>
+    <row r="37" ht="50.1" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="39" orientation="portrait" r:id="rId1"/>
@@ -2836,12 +2837,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Work on FMEA of RTx Controller Schematic
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-14025" yWindow="855" windowWidth="19440" windowHeight="10035"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="198">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -418,13 +418,208 @@
   </si>
   <si>
     <t>Use Active Pull-Down on GPIO (Recalculate external pull-down value)</t>
+  </si>
+  <si>
+    <t>Controller Board</t>
+  </si>
+  <si>
+    <t>Analog-to-Digital Converters</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>coupling on +3.3V</t>
+  </si>
+  <si>
+    <t>coupling on +5V</t>
+  </si>
+  <si>
+    <t>coupling on +5VREF</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>SDO is open</t>
+  </si>
+  <si>
+    <t>SPI/MISO3 is floating</t>
+  </si>
+  <si>
+    <t>Low-Pass Filters for Feedback ADCs</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>OPAMP1-A</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>OPAMP1-B</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>OPAMP2-A</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>OPAMP2-B</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>Ethernet</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>C53</t>
+  </si>
+  <si>
+    <t>C56</t>
+  </si>
+  <si>
+    <t>C57</t>
+  </si>
+  <si>
+    <t>C58</t>
+  </si>
+  <si>
+    <t>C59</t>
+  </si>
+  <si>
+    <t>C60</t>
+  </si>
+  <si>
+    <t>C61</t>
+  </si>
+  <si>
+    <t>C62</t>
+  </si>
+  <si>
+    <t>C63</t>
+  </si>
+  <si>
+    <t>C64</t>
+  </si>
+  <si>
+    <t>C65</t>
+  </si>
+  <si>
+    <t>C66</t>
+  </si>
+  <si>
+    <t>C67</t>
+  </si>
+  <si>
+    <t>C68</t>
+  </si>
+  <si>
+    <t>C69</t>
+  </si>
+  <si>
+    <t>C70</t>
+  </si>
+  <si>
+    <t>C71</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +652,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="22"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
@@ -464,15 +674,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -480,11 +696,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -515,29 +766,39 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -551,10 +812,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -572,10 +833,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -589,10 +850,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -610,10 +871,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -627,10 +888,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -648,10 +909,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -665,10 +926,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -686,49 +947,49 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -887,6 +1148,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -921,6 +1183,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1096,14 +1359,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M132"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
@@ -1113,24 +1376,24 @@
     <col min="8" max="9" width="25.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26.5703125" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="46.5">
+    <row r="2" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="46.5">
+    <row r="3" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="2:13" ht="28.5">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:13" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="31.5" customHeight="1">
+    <row r="5" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1168,7 +1431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>1</v>
       </c>
@@ -1202,7 +1465,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>2</v>
       </c>
@@ -1236,7 +1499,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>3</v>
       </c>
@@ -1270,7 +1533,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>4</v>
       </c>
@@ -1304,7 +1567,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>5</v>
       </c>
@@ -1340,7 +1603,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>6</v>
       </c>
@@ -1376,7 +1639,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>7</v>
       </c>
@@ -1412,7 +1675,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>8</v>
       </c>
@@ -1448,7 +1711,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="30">
+    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>9</v>
       </c>
@@ -1484,7 +1747,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>10</v>
       </c>
@@ -1520,7 +1783,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>11</v>
       </c>
@@ -1556,7 +1819,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="30">
+    <row r="17" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>12</v>
       </c>
@@ -1592,7 +1855,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="30">
+    <row r="18" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>13</v>
       </c>
@@ -1630,7 +1893,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="75">
+    <row r="19" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>14</v>
       </c>
@@ -1666,7 +1929,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="30">
+    <row r="20" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>15</v>
       </c>
@@ -1702,7 +1965,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="30">
+    <row r="21" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>16</v>
       </c>
@@ -1738,7 +2001,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>17</v>
       </c>
@@ -1772,7 +2035,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>18</v>
       </c>
@@ -1806,7 +2069,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>19</v>
       </c>
@@ -1840,7 +2103,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <v>20</v>
       </c>
@@ -1874,7 +2137,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="15.75" customHeight="1">
+    <row r="26" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>21</v>
       </c>
@@ -1912,7 +2175,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="30">
+    <row r="27" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>22</v>
       </c>
@@ -1950,7 +2213,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="30">
+    <row r="28" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>23</v>
       </c>
@@ -1986,7 +2249,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="30">
+    <row r="29" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>24</v>
       </c>
@@ -2022,7 +2285,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="30">
+    <row r="30" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>25</v>
       </c>
@@ -2060,7 +2323,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="30">
+    <row r="31" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>26</v>
       </c>
@@ -2098,7 +2361,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>27</v>
       </c>
@@ -2136,7 +2399,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="30">
+    <row r="33" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>28</v>
       </c>
@@ -2174,7 +2437,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="2:13">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <v>29</v>
       </c>
@@ -2208,7 +2471,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="30">
+    <row r="35" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <v>30</v>
       </c>
@@ -2246,7 +2509,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="2:13">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <v>31</v>
       </c>
@@ -2284,7 +2547,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="2:13">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
         <v>32</v>
       </c>
@@ -2322,7 +2585,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="30">
+    <row r="38" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <v>33</v>
       </c>
@@ -2360,7 +2623,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="2:13" ht="30">
+    <row r="39" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>34</v>
       </c>
@@ -2398,7 +2661,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="30">
+    <row r="40" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <v>35</v>
       </c>
@@ -2436,7 +2699,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="2:13">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
         <v>36</v>
       </c>
@@ -2474,8 +2737,992 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="46.5">
-      <c r="B47" s="5"/>
+    <row r="47" spans="2:13" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B49" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>38</v>
+      </c>
+      <c r="C52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>39</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" t="s">
+        <v>117</v>
+      </c>
+      <c r="F54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E57" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>44</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" t="s">
+        <v>117</v>
+      </c>
+      <c r="F58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>46</v>
+      </c>
+      <c r="C60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" t="s">
+        <v>117</v>
+      </c>
+      <c r="F60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>47</v>
+      </c>
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" t="s">
+        <v>117</v>
+      </c>
+      <c r="F61" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>48</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" t="s">
+        <v>117</v>
+      </c>
+      <c r="F62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>49</v>
+      </c>
+      <c r="C63" t="s">
+        <v>142</v>
+      </c>
+      <c r="D63" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" t="s">
+        <v>143</v>
+      </c>
+      <c r="G63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B66" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M67" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>50</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>51</v>
+      </c>
+      <c r="C69" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>52</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" t="s">
+        <v>138</v>
+      </c>
+      <c r="E70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>53</v>
+      </c>
+      <c r="C71" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>146</v>
+      </c>
+      <c r="D72" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>56</v>
+      </c>
+      <c r="C74" t="s">
+        <v>148</v>
+      </c>
+      <c r="D74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>57</v>
+      </c>
+      <c r="C75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>58</v>
+      </c>
+      <c r="C76" t="s">
+        <v>53</v>
+      </c>
+      <c r="D76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>59</v>
+      </c>
+      <c r="C77" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" t="s">
+        <v>138</v>
+      </c>
+      <c r="E77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>60</v>
+      </c>
+      <c r="C78" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" t="s">
+        <v>138</v>
+      </c>
+      <c r="E78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>150</v>
+      </c>
+      <c r="D79" t="s">
+        <v>81</v>
+      </c>
+      <c r="E79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>62</v>
+      </c>
+      <c r="C80" t="s">
+        <v>167</v>
+      </c>
+      <c r="D80" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>63</v>
+      </c>
+      <c r="C81" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>64</v>
+      </c>
+      <c r="C82" t="s">
+        <v>152</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>65</v>
+      </c>
+      <c r="C83" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>66</v>
+      </c>
+      <c r="C84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>67</v>
+      </c>
+      <c r="C85" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" t="s">
+        <v>138</v>
+      </c>
+      <c r="E85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>68</v>
+      </c>
+      <c r="C86" t="s">
+        <v>58</v>
+      </c>
+      <c r="D86" t="s">
+        <v>138</v>
+      </c>
+      <c r="E86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>69</v>
+      </c>
+      <c r="C87" t="s">
+        <v>154</v>
+      </c>
+      <c r="D87" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>70</v>
+      </c>
+      <c r="C88" t="s">
+        <v>155</v>
+      </c>
+      <c r="D88" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>71</v>
+      </c>
+      <c r="C89" t="s">
+        <v>156</v>
+      </c>
+      <c r="D89" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>72</v>
+      </c>
+      <c r="C90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D90" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>73</v>
+      </c>
+      <c r="C91" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>74</v>
+      </c>
+      <c r="C92" t="s">
+        <v>159</v>
+      </c>
+      <c r="D92" t="s">
+        <v>138</v>
+      </c>
+      <c r="E92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>75</v>
+      </c>
+      <c r="C93" t="s">
+        <v>160</v>
+      </c>
+      <c r="D93" t="s">
+        <v>138</v>
+      </c>
+      <c r="E93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>76</v>
+      </c>
+      <c r="C94" t="s">
+        <v>161</v>
+      </c>
+      <c r="D94" t="s">
+        <v>138</v>
+      </c>
+      <c r="E94" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>77</v>
+      </c>
+      <c r="C95" t="s">
+        <v>162</v>
+      </c>
+      <c r="D95" t="s">
+        <v>81</v>
+      </c>
+      <c r="E95" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>78</v>
+      </c>
+      <c r="C96" t="s">
+        <v>163</v>
+      </c>
+      <c r="D96" t="s">
+        <v>81</v>
+      </c>
+      <c r="E96" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>79</v>
+      </c>
+      <c r="C97" t="s">
+        <v>164</v>
+      </c>
+      <c r="D97" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>80</v>
+      </c>
+      <c r="C98" t="s">
+        <v>165</v>
+      </c>
+      <c r="D98" t="s">
+        <v>81</v>
+      </c>
+      <c r="E98" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>81</v>
+      </c>
+      <c r="C99" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B102" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F103" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I103" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J103" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K103" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L103" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M103" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>82</v>
+      </c>
+      <c r="C104" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>83</v>
+      </c>
+      <c r="C105" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>84</v>
+      </c>
+      <c r="C106" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>85</v>
+      </c>
+      <c r="C107" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>86</v>
+      </c>
+      <c r="C108" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>87</v>
+      </c>
+      <c r="C109" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>88</v>
+      </c>
+      <c r="C110" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>89</v>
+      </c>
+      <c r="C111" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>90</v>
+      </c>
+      <c r="C112" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>91</v>
+      </c>
+      <c r="C113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>92</v>
+      </c>
+      <c r="C114" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>93</v>
+      </c>
+      <c r="C115" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>94</v>
+      </c>
+      <c r="C116" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>95</v>
+      </c>
+      <c r="C117" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>96</v>
+      </c>
+      <c r="C118" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>97</v>
+      </c>
+      <c r="C119" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>98</v>
+      </c>
+      <c r="C120" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>99</v>
+      </c>
+      <c r="C121" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>100</v>
+      </c>
+      <c r="C122" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>101</v>
+      </c>
+      <c r="C123" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>102</v>
+      </c>
+      <c r="C124" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>103</v>
+      </c>
+      <c r="C125" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>104</v>
+      </c>
+      <c r="C126" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>105</v>
+      </c>
+      <c r="C127" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>106</v>
+      </c>
+      <c r="C128" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>107</v>
+      </c>
+      <c r="C129" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>108</v>
+      </c>
+      <c r="C130" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>109</v>
+      </c>
+      <c r="C131" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>110</v>
+      </c>
+      <c r="C132" t="s">
+        <v>197</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2487,14 +3734,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="58.5703125" customWidth="1"/>
@@ -2507,7 +3754,7 @@
     <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="50.1" customHeight="1">
+    <row r="3" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
@@ -2516,7 +3763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="50.1" customHeight="1">
+    <row r="4" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2545,7 +3792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="50.1" customHeight="1">
+    <row r="5" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
@@ -2574,7 +3821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="50.1" customHeight="1">
+    <row r="6" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2603,7 +3850,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="50.1" customHeight="1">
+    <row r="7" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2632,7 +3879,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="50.1" customHeight="1">
+    <row r="8" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +3908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="50.1" customHeight="1">
+    <row r="9" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
@@ -2690,14 +3937,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="50.1" customHeight="1"/>
-    <row r="11" spans="2:13" ht="50.1" customHeight="1"/>
-    <row r="12" spans="2:13" ht="50.1" customHeight="1">
+    <row r="10" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="50.1" customHeight="1">
+    <row r="13" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2705,7 +3952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="50.1" customHeight="1">
+    <row r="14" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
@@ -2713,7 +3960,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="50.1" customHeight="1">
+    <row r="15" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
@@ -2721,7 +3968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="50.1" customHeight="1">
+    <row r="16" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
@@ -2729,7 +3976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="50.1" customHeight="1">
+    <row r="17" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
@@ -2737,7 +3984,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="50.1" customHeight="1">
+    <row r="18" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2745,7 +3992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="50.1" customHeight="1">
+    <row r="19" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2753,14 +4000,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="50.1" customHeight="1"/>
-    <row r="21" spans="2:3" ht="50.1" customHeight="1"/>
-    <row r="22" spans="2:3" ht="50.1" customHeight="1">
+    <row r="20" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="50.1" customHeight="1">
+    <row r="23" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -2768,7 +4015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="50.1" customHeight="1">
+    <row r="24" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>1</v>
       </c>
@@ -2776,7 +4023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="50.1" customHeight="1">
+    <row r="25" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>2</v>
       </c>
@@ -2784,7 +4031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="50.1" customHeight="1">
+    <row r="26" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>3</v>
       </c>
@@ -2792,7 +4039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="50.1" customHeight="1">
+    <row r="27" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>4</v>
       </c>
@@ -2800,7 +4047,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="50.1" customHeight="1">
+    <row r="28" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <v>5</v>
       </c>
@@ -2808,7 +4055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="50.1" customHeight="1">
+    <row r="29" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <v>6</v>
       </c>
@@ -2816,14 +4063,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="50.1" customHeight="1"/>
-    <row r="31" spans="2:3" ht="50.1" customHeight="1"/>
-    <row r="32" spans="2:3" ht="50.1" customHeight="1"/>
-    <row r="33" ht="50.1" customHeight="1"/>
-    <row r="34" ht="50.1" customHeight="1"/>
-    <row r="35" ht="50.1" customHeight="1"/>
-    <row r="36" ht="50.1" customHeight="1"/>
-    <row r="37" ht="50.1" customHeight="1"/>
+    <row r="30" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="39" orientation="portrait" r:id="rId1"/>
@@ -2837,12 +4084,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates made to FMEA.
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="232">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -438,15 +438,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>coupling on +3.3V</t>
-  </si>
-  <si>
-    <t>coupling on +5V</t>
-  </si>
-  <si>
-    <t>coupling on +5VREF</t>
-  </si>
-  <si>
     <t>R20</t>
   </si>
   <si>
@@ -613,13 +604,124 @@
   </si>
   <si>
     <t>C71</t>
+  </si>
+  <si>
+    <t>Ethernet PHY</t>
+  </si>
+  <si>
+    <t>Ethernet Connector</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>C50</t>
+  </si>
+  <si>
+    <t>C51</t>
+  </si>
+  <si>
+    <t>PoE</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>C49</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>R_LED1</t>
+  </si>
+  <si>
+    <t>POE</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>short out +5VREF</t>
+  </si>
+  <si>
+    <t>short out +5V</t>
+  </si>
+  <si>
+    <t>short out +3.3V</t>
+  </si>
+  <si>
+    <t>TD+,TD- outputs would be useless</t>
+  </si>
+  <si>
+    <t>RBIAS floating</t>
+  </si>
+  <si>
+    <t>RESERVED would float</t>
+  </si>
+  <si>
+    <t>PFBOUT, PFBIN1, PFBIN2 grounded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +771,13 @@
     <font>
       <sz val="22"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -777,11 +886,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -986,9 +1099,6 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1011,63 +1121,63 @@
     <tableColumn id="2" name="Item" dataDxfId="31"/>
     <tableColumn id="3" name="Potential failure mode" dataDxfId="30"/>
     <tableColumn id="4" name="Potential cause(s)" dataDxfId="29"/>
-    <tableColumn id="6" name="local effects of failure" dataDxfId="28"/>
-    <tableColumn id="7" name="next higher level effect" dataDxfId="27"/>
-    <tableColumn id="8" name="system level end effect" dataDxfId="26"/>
-    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="25"/>
-    <tableColumn id="10" name="(S) Severity" dataDxfId="24"/>
-    <tableColumn id="12" name="Risk Level" dataDxfId="23"/>
-    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="22"/>
-    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="21"/>
+    <tableColumn id="6" name="local effects of failure" dataDxfId="0"/>
+    <tableColumn id="7" name="next higher level effect" dataDxfId="28"/>
+    <tableColumn id="8" name="system level end effect" dataDxfId="27"/>
+    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="26"/>
+    <tableColumn id="10" name="(S) Severity" dataDxfId="25"/>
+    <tableColumn id="12" name="Risk Level" dataDxfId="24"/>
+    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="23"/>
+    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B4:C9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="18"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="17"/>
+    <tableColumn id="1" name="Rating" dataDxfId="19"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B13:C19"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="14"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="13"/>
+    <tableColumn id="1" name="Rating" dataDxfId="15"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B23:C29"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="10"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="9"/>
+    <tableColumn id="1" name="Rating" dataDxfId="11"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="G4:M9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Probability \ Severity" dataDxfId="6"/>
-    <tableColumn id="2" name="I" dataDxfId="5"/>
-    <tableColumn id="3" name="II" dataDxfId="4"/>
-    <tableColumn id="4" name="III" dataDxfId="3"/>
-    <tableColumn id="5" name="IV" dataDxfId="2"/>
-    <tableColumn id="6" name="V" dataDxfId="1"/>
-    <tableColumn id="7" name="VI" dataDxfId="0"/>
+    <tableColumn id="1" name="Probability \ Severity" dataDxfId="7"/>
+    <tableColumn id="2" name="I" dataDxfId="6"/>
+    <tableColumn id="3" name="II" dataDxfId="5"/>
+    <tableColumn id="4" name="III" dataDxfId="4"/>
+    <tableColumn id="5" name="IV" dataDxfId="3"/>
+    <tableColumn id="6" name="V" dataDxfId="2"/>
+    <tableColumn id="7" name="VI" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1360,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M132"/>
+  <dimension ref="B2:M185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,11 +1497,13 @@
     </row>
     <row r="3" spans="2:13" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B3" s="5"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:13" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="15" t="s">
         <v>47</v>
       </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -1893,7 +2005,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <v>14</v>
       </c>
@@ -2737,15 +2849,35 @@
         <v>121</v>
       </c>
     </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F46" s="1"/>
+    </row>
     <row r="47" spans="2:13" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="15" t="s">
         <v>133</v>
       </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B49" s="16" t="s">
         <v>134</v>
       </c>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
@@ -2792,6 +2924,7 @@
       <c r="C51" t="s">
         <v>135</v>
       </c>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -2806,8 +2939,8 @@
       <c r="E52" t="s">
         <v>117</v>
       </c>
-      <c r="F52" t="s">
-        <v>141</v>
+      <c r="F52" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
@@ -2823,8 +2956,8 @@
       <c r="E53" t="s">
         <v>117</v>
       </c>
-      <c r="F53" t="s">
-        <v>140</v>
+      <c r="F53" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
@@ -2840,8 +2973,8 @@
       <c r="E54" t="s">
         <v>117</v>
       </c>
-      <c r="F54" t="s">
-        <v>139</v>
+      <c r="F54" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
@@ -2851,6 +2984,7 @@
       <c r="C55" t="s">
         <v>136</v>
       </c>
+      <c r="F55" s="1"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56">
@@ -2865,8 +2999,8 @@
       <c r="E56" t="s">
         <v>117</v>
       </c>
-      <c r="F56" t="s">
-        <v>141</v>
+      <c r="F56" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
@@ -2882,8 +3016,8 @@
       <c r="E57" t="s">
         <v>117</v>
       </c>
-      <c r="F57" t="s">
-        <v>140</v>
+      <c r="F57" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
@@ -2899,8 +3033,8 @@
       <c r="E58" t="s">
         <v>117</v>
       </c>
-      <c r="F58" t="s">
-        <v>139</v>
+      <c r="F58" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
@@ -2910,6 +3044,7 @@
       <c r="C59" t="s">
         <v>137</v>
       </c>
+      <c r="F59" s="1"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60">
@@ -2924,8 +3059,8 @@
       <c r="E60" t="s">
         <v>117</v>
       </c>
-      <c r="F60" t="s">
-        <v>141</v>
+      <c r="F60" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
@@ -2941,8 +3076,8 @@
       <c r="E61" t="s">
         <v>117</v>
       </c>
-      <c r="F61" t="s">
-        <v>140</v>
+      <c r="F61" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
@@ -2958,8 +3093,8 @@
       <c r="E62" t="s">
         <v>117</v>
       </c>
-      <c r="F62" t="s">
-        <v>139</v>
+      <c r="F62" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.25">
@@ -2967,7 +3102,7 @@
         <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D63" t="s">
         <v>138</v>
@@ -2975,17 +3110,24 @@
       <c r="E63" t="s">
         <v>123</v>
       </c>
-      <c r="F63" t="s">
-        <v>143</v>
+      <c r="F63" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="G63" t="s">
-        <v>144</v>
-      </c>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F65" s="1"/>
     </row>
     <row r="66" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B66" s="16" t="s">
-        <v>145</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="F66" s="1"/>
     </row>
     <row r="67" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="14" t="s">
@@ -3038,6 +3180,7 @@
       <c r="E68" t="s">
         <v>123</v>
       </c>
+      <c r="F68" s="1"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69">
@@ -3052,6 +3195,7 @@
       <c r="E69" t="s">
         <v>123</v>
       </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70">
@@ -3066,6 +3210,7 @@
       <c r="E70" t="s">
         <v>123</v>
       </c>
+      <c r="F70" s="1"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71">
@@ -3080,13 +3225,14 @@
       <c r="E71" t="s">
         <v>117</v>
       </c>
+      <c r="F71" s="1"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D72" t="s">
         <v>81</v>
@@ -3094,13 +3240,14 @@
       <c r="E72" t="s">
         <v>117</v>
       </c>
+      <c r="F72" s="1"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D73" t="s">
         <v>81</v>
@@ -3108,13 +3255,14 @@
       <c r="E73" t="s">
         <v>117</v>
       </c>
+      <c r="F73" s="1"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D74" t="s">
         <v>81</v>
@@ -3122,14 +3270,16 @@
       <c r="E74" t="s">
         <v>117</v>
       </c>
+      <c r="F74" s="1"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>57</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="F75" s="1"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76">
@@ -3144,6 +3294,7 @@
       <c r="E76" t="s">
         <v>123</v>
       </c>
+      <c r="F76" s="1"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B77">
@@ -3158,6 +3309,7 @@
       <c r="E77" t="s">
         <v>123</v>
       </c>
+      <c r="F77" s="1"/>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B78">
@@ -3172,13 +3324,14 @@
       <c r="E78" t="s">
         <v>123</v>
       </c>
+      <c r="F78" s="1"/>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D79" t="s">
         <v>81</v>
@@ -3186,13 +3339,14 @@
       <c r="E79" t="s">
         <v>117</v>
       </c>
+      <c r="F79" s="1"/>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D80" t="s">
         <v>81</v>
@@ -3200,13 +3354,14 @@
       <c r="E80" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>63</v>
       </c>
       <c r="C81" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D81" t="s">
         <v>81</v>
@@ -3214,13 +3369,14 @@
       <c r="E81" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>64</v>
       </c>
       <c r="C82" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D82" t="s">
         <v>81</v>
@@ -3228,16 +3384,18 @@
       <c r="E82" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>65</v>
       </c>
       <c r="C83" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>66</v>
       </c>
@@ -3250,8 +3408,9 @@
       <c r="E84" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>67</v>
       </c>
@@ -3264,8 +3423,9 @@
       <c r="E85" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>68</v>
       </c>
@@ -3278,13 +3438,14 @@
       <c r="E86" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>69</v>
       </c>
       <c r="C87" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D87" t="s">
         <v>81</v>
@@ -3292,13 +3453,14 @@
       <c r="E87" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>70</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D88" t="s">
         <v>81</v>
@@ -3306,13 +3468,14 @@
       <c r="E88" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>71</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D89" t="s">
         <v>81</v>
@@ -3320,13 +3483,14 @@
       <c r="E89" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D90" t="s">
         <v>81</v>
@@ -3334,21 +3498,23 @@
       <c r="E90" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>74</v>
       </c>
       <c r="C92" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D92" t="s">
         <v>138</v>
@@ -3356,13 +3522,14 @@
       <c r="E92" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>75</v>
       </c>
       <c r="C93" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D93" t="s">
         <v>138</v>
@@ -3370,13 +3537,14 @@
       <c r="E93" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="1"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>76</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D94" t="s">
         <v>138</v>
@@ -3384,13 +3552,14 @@
       <c r="E94" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>77</v>
       </c>
       <c r="C95" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D95" t="s">
         <v>81</v>
@@ -3398,13 +3567,14 @@
       <c r="E95" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>78</v>
       </c>
       <c r="C96" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D96" t="s">
         <v>81</v>
@@ -3412,13 +3582,14 @@
       <c r="E96" t="s">
         <v>117</v>
       </c>
+      <c r="F96" s="1"/>
     </row>
     <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>79</v>
       </c>
       <c r="C97" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D97" t="s">
         <v>81</v>
@@ -3426,13 +3597,14 @@
       <c r="E97" t="s">
         <v>117</v>
       </c>
+      <c r="F97" s="1"/>
     </row>
     <row r="98" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>80</v>
       </c>
       <c r="C98" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D98" t="s">
         <v>81</v>
@@ -3440,289 +3612,1028 @@
       <c r="E98" t="s">
         <v>117</v>
       </c>
+      <c r="F98" s="1"/>
     </row>
     <row r="99" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>81</v>
       </c>
       <c r="C99" t="s">
-        <v>166</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="F99" s="1"/>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F100" s="1"/>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F101" s="1"/>
     </row>
     <row r="102" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B102" s="16" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="103" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F102" s="1"/>
+    </row>
+    <row r="103" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B103" s="16"/>
+      <c r="F103" s="1"/>
+    </row>
+    <row r="104" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B104" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F104" s="1"/>
+    </row>
+    <row r="105" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="C105" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D105" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E103" s="12" t="s">
+      <c r="E105" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F105" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="G105" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H103" s="12" t="s">
+      <c r="H105" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I103" s="12" t="s">
+      <c r="I105" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J103" s="12" t="s">
+      <c r="J105" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K103" s="12" t="s">
+      <c r="K105" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L103" s="12" t="s">
+      <c r="L105" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M103" s="13" t="s">
+      <c r="M105" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B104">
+    <row r="106" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B106">
         <v>82</v>
       </c>
-      <c r="C104" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B105">
-        <v>83</v>
-      </c>
-      <c r="C105" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B106">
-        <v>84</v>
-      </c>
       <c r="C106" t="s">
-        <v>171</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="F106" s="1"/>
     </row>
     <row r="107" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B107">
+        <v>83</v>
+      </c>
+      <c r="C107" t="s">
+        <v>167</v>
+      </c>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>84</v>
+      </c>
+      <c r="C108" t="s">
+        <v>168</v>
+      </c>
+      <c r="D108" t="s">
+        <v>138</v>
+      </c>
+      <c r="E108" t="s">
+        <v>123</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B109">
         <v>85</v>
       </c>
-      <c r="C107" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B108">
-        <v>86</v>
-      </c>
-      <c r="C108" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B109">
-        <v>87</v>
-      </c>
       <c r="C109" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="D109" t="s">
+        <v>138</v>
+      </c>
+      <c r="E109" t="s">
+        <v>123</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="110" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C110" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="D110" t="s">
+        <v>138</v>
+      </c>
+      <c r="E110" t="s">
+        <v>123</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="111" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C111" t="s">
-        <v>176</v>
+        <v>171</v>
+      </c>
+      <c r="D111" t="s">
+        <v>138</v>
+      </c>
+      <c r="E111" t="s">
+        <v>123</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B112">
+        <v>88</v>
+      </c>
+      <c r="C112" t="s">
+        <v>172</v>
+      </c>
+      <c r="D112" t="s">
+        <v>138</v>
+      </c>
+      <c r="E112" t="s">
+        <v>123</v>
+      </c>
+      <c r="F112" s="1"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>89</v>
+      </c>
+      <c r="C113" t="s">
+        <v>173</v>
+      </c>
+      <c r="D113" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113" t="s">
+        <v>123</v>
+      </c>
+      <c r="F113" s="1"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114">
         <v>90</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C114" t="s">
+        <v>174</v>
+      </c>
+      <c r="D114" t="s">
+        <v>138</v>
+      </c>
+      <c r="E114" t="s">
+        <v>123</v>
+      </c>
+      <c r="F114" s="1"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>91</v>
+      </c>
+      <c r="C115" t="s">
+        <v>175</v>
+      </c>
+      <c r="D115" t="s">
+        <v>138</v>
+      </c>
+      <c r="E115" t="s">
+        <v>123</v>
+      </c>
+      <c r="F115" s="1"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>92</v>
+      </c>
+      <c r="C116" t="s">
+        <v>176</v>
+      </c>
+      <c r="D116" t="s">
+        <v>138</v>
+      </c>
+      <c r="E116" t="s">
+        <v>123</v>
+      </c>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>93</v>
+      </c>
+      <c r="C117" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113">
-        <v>91</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="D117" t="s">
+        <v>81</v>
+      </c>
+      <c r="E117" t="s">
+        <v>117</v>
+      </c>
+      <c r="F117" s="1"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>94</v>
+      </c>
+      <c r="C118" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114">
-        <v>92</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="D118" t="s">
+        <v>81</v>
+      </c>
+      <c r="E118" t="s">
+        <v>117</v>
+      </c>
+      <c r="F118" s="1"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>95</v>
+      </c>
+      <c r="C119" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115">
-        <v>93</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="D119" t="s">
+        <v>81</v>
+      </c>
+      <c r="E119" t="s">
+        <v>117</v>
+      </c>
+      <c r="F119" s="1"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>96</v>
+      </c>
+      <c r="C120" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116">
-        <v>94</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="D120" t="s">
+        <v>81</v>
+      </c>
+      <c r="E120" t="s">
+        <v>117</v>
+      </c>
+      <c r="F120" s="1"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>97</v>
+      </c>
+      <c r="C121" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117">
-        <v>95</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="D121" t="s">
+        <v>81</v>
+      </c>
+      <c r="E121" t="s">
+        <v>117</v>
+      </c>
+      <c r="F121" s="1"/>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>98</v>
+      </c>
+      <c r="C122" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118">
-        <v>96</v>
-      </c>
-      <c r="C118" t="s">
+      <c r="D122" t="s">
+        <v>81</v>
+      </c>
+      <c r="E122" t="s">
+        <v>117</v>
+      </c>
+      <c r="F122" s="1"/>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>99</v>
+      </c>
+      <c r="C123" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119">
-        <v>97</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D123" t="s">
+        <v>81</v>
+      </c>
+      <c r="E123" t="s">
+        <v>117</v>
+      </c>
+      <c r="F123" s="1"/>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>100</v>
+      </c>
+      <c r="C124" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120">
-        <v>98</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="D124" t="s">
+        <v>81</v>
+      </c>
+      <c r="E124" t="s">
+        <v>117</v>
+      </c>
+      <c r="F124" s="1"/>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>101</v>
+      </c>
+      <c r="C125" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121">
-        <v>99</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="D125" t="s">
+        <v>81</v>
+      </c>
+      <c r="E125" t="s">
+        <v>117</v>
+      </c>
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>102</v>
+      </c>
+      <c r="C126" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122">
-        <v>100</v>
-      </c>
-      <c r="C122" t="s">
+      <c r="D126" t="s">
+        <v>81</v>
+      </c>
+      <c r="E126" t="s">
+        <v>117</v>
+      </c>
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>103</v>
+      </c>
+      <c r="C127" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123">
-        <v>101</v>
-      </c>
-      <c r="C123" t="s">
+      <c r="D127" t="s">
+        <v>81</v>
+      </c>
+      <c r="E127" t="s">
+        <v>117</v>
+      </c>
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>104</v>
+      </c>
+      <c r="C128" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124">
-        <v>102</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="D128" t="s">
+        <v>81</v>
+      </c>
+      <c r="E128" t="s">
+        <v>117</v>
+      </c>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>105</v>
+      </c>
+      <c r="C129" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125">
-        <v>103</v>
-      </c>
-      <c r="C125" t="s">
+      <c r="D129" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" t="s">
+        <v>117</v>
+      </c>
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>106</v>
+      </c>
+      <c r="C130" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B126">
-        <v>104</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="D130" t="s">
+        <v>81</v>
+      </c>
+      <c r="E130" t="s">
+        <v>117</v>
+      </c>
+      <c r="F130" s="1"/>
+    </row>
+    <row r="131" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>107</v>
+      </c>
+      <c r="C131" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>105</v>
-      </c>
-      <c r="C127" t="s">
+      <c r="D131" t="s">
+        <v>81</v>
+      </c>
+      <c r="E131" t="s">
+        <v>117</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="132" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>108</v>
+      </c>
+      <c r="C132" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128">
-        <v>106</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="D132" t="s">
+        <v>81</v>
+      </c>
+      <c r="E132" t="s">
+        <v>117</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="133" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>109</v>
+      </c>
+      <c r="C133" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129">
-        <v>107</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="D133" t="s">
+        <v>81</v>
+      </c>
+      <c r="E133" t="s">
+        <v>117</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="134" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>110</v>
+      </c>
+      <c r="C134" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130">
-        <v>108</v>
-      </c>
-      <c r="C130" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131">
-        <v>109</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="D134" t="s">
+        <v>81</v>
+      </c>
+      <c r="E134" t="s">
+        <v>117</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B136" s="17" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B132">
-        <v>110</v>
-      </c>
-      <c r="C132" t="s">
+      <c r="F136" s="1"/>
+    </row>
+    <row r="137" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E137" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F137" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G137" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H137" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I137" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J137" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K137" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L137" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M137" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>111</v>
+      </c>
+      <c r="C138" t="s">
         <v>197</v>
       </c>
+      <c r="F138" s="1"/>
+    </row>
+    <row r="139" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>112</v>
+      </c>
+      <c r="C139" t="s">
+        <v>198</v>
+      </c>
+      <c r="D139" t="s">
+        <v>138</v>
+      </c>
+      <c r="E139" t="s">
+        <v>123</v>
+      </c>
+      <c r="F139" s="1"/>
+    </row>
+    <row r="140" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>113</v>
+      </c>
+      <c r="C140" t="s">
+        <v>199</v>
+      </c>
+      <c r="D140" t="s">
+        <v>138</v>
+      </c>
+      <c r="E140" t="s">
+        <v>123</v>
+      </c>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>114</v>
+      </c>
+      <c r="C141" t="s">
+        <v>200</v>
+      </c>
+      <c r="D141" t="s">
+        <v>138</v>
+      </c>
+      <c r="E141" t="s">
+        <v>123</v>
+      </c>
+      <c r="F141" s="1"/>
+    </row>
+    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>115</v>
+      </c>
+      <c r="C142" t="s">
+        <v>201</v>
+      </c>
+      <c r="D142" t="s">
+        <v>138</v>
+      </c>
+      <c r="E142" t="s">
+        <v>123</v>
+      </c>
+      <c r="F142" s="1"/>
+    </row>
+    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>116</v>
+      </c>
+      <c r="C143" t="s">
+        <v>202</v>
+      </c>
+      <c r="D143" t="s">
+        <v>81</v>
+      </c>
+      <c r="E143" t="s">
+        <v>117</v>
+      </c>
+      <c r="F143" s="1"/>
+    </row>
+    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>117</v>
+      </c>
+      <c r="C144" t="s">
+        <v>203</v>
+      </c>
+      <c r="D144" t="s">
+        <v>81</v>
+      </c>
+      <c r="E144" t="s">
+        <v>117</v>
+      </c>
+      <c r="F144" s="1"/>
+    </row>
+    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>118</v>
+      </c>
+      <c r="C145" t="s">
+        <v>204</v>
+      </c>
+      <c r="D145" t="s">
+        <v>81</v>
+      </c>
+      <c r="E145" t="s">
+        <v>117</v>
+      </c>
+      <c r="F145" s="1"/>
+    </row>
+    <row r="146" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>119</v>
+      </c>
+      <c r="C146" t="s">
+        <v>205</v>
+      </c>
+      <c r="D146" t="s">
+        <v>81</v>
+      </c>
+      <c r="E146" t="s">
+        <v>117</v>
+      </c>
+      <c r="F146" s="1"/>
+    </row>
+    <row r="147" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F147" s="1"/>
+    </row>
+    <row r="148" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B148" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F148" s="1"/>
+    </row>
+    <row r="149" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D149" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E149" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F149" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H149" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I149" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J149" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K149" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L149" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M149" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>120</v>
+      </c>
+      <c r="C150" t="s">
+        <v>207</v>
+      </c>
+      <c r="F150" s="1"/>
+    </row>
+    <row r="151" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>120</v>
+      </c>
+      <c r="C151" t="s">
+        <v>208</v>
+      </c>
+      <c r="F151" s="1"/>
+    </row>
+    <row r="152" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>120</v>
+      </c>
+      <c r="C152" t="s">
+        <v>209</v>
+      </c>
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>120</v>
+      </c>
+      <c r="C153" t="s">
+        <v>210</v>
+      </c>
+      <c r="F153" s="1"/>
+    </row>
+    <row r="154" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>120</v>
+      </c>
+      <c r="C154" t="s">
+        <v>211</v>
+      </c>
+      <c r="D154" t="s">
+        <v>81</v>
+      </c>
+      <c r="E154" t="s">
+        <v>117</v>
+      </c>
+      <c r="F154" s="1"/>
+    </row>
+    <row r="155" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>120</v>
+      </c>
+      <c r="C155" t="s">
+        <v>212</v>
+      </c>
+      <c r="D155" t="s">
+        <v>81</v>
+      </c>
+      <c r="E155" t="s">
+        <v>117</v>
+      </c>
+      <c r="F155" s="1"/>
+    </row>
+    <row r="156" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>120</v>
+      </c>
+      <c r="C156" t="s">
+        <v>213</v>
+      </c>
+      <c r="D156" t="s">
+        <v>81</v>
+      </c>
+      <c r="E156" t="s">
+        <v>117</v>
+      </c>
+      <c r="F156" s="1"/>
+    </row>
+    <row r="157" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>120</v>
+      </c>
+      <c r="C157" t="s">
+        <v>214</v>
+      </c>
+      <c r="F157" s="1"/>
+    </row>
+    <row r="158" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>120</v>
+      </c>
+      <c r="C158" t="s">
+        <v>215</v>
+      </c>
+      <c r="F158" s="1"/>
+    </row>
+    <row r="159" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>120</v>
+      </c>
+      <c r="C159" t="s">
+        <v>216</v>
+      </c>
+      <c r="F159" s="1"/>
+    </row>
+    <row r="160" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>120</v>
+      </c>
+      <c r="C160" t="s">
+        <v>217</v>
+      </c>
+      <c r="F160" s="1"/>
+    </row>
+    <row r="161" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F161" s="1"/>
+    </row>
+    <row r="162" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F162" s="1"/>
+    </row>
+    <row r="163" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B163" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F163" s="1"/>
+    </row>
+    <row r="164" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C164" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F164" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G164" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H164" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I164" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J164" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K164" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L164" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M164" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="165" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>121</v>
+      </c>
+      <c r="C165" t="s">
+        <v>219</v>
+      </c>
+      <c r="D165" t="s">
+        <v>138</v>
+      </c>
+      <c r="E165" t="s">
+        <v>123</v>
+      </c>
+      <c r="F165" s="1"/>
+    </row>
+    <row r="166" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>122</v>
+      </c>
+      <c r="C166" t="s">
+        <v>220</v>
+      </c>
+      <c r="D166" t="s">
+        <v>138</v>
+      </c>
+      <c r="E166" t="s">
+        <v>123</v>
+      </c>
+      <c r="F166" s="1"/>
+    </row>
+    <row r="167" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>123</v>
+      </c>
+      <c r="C167" t="s">
+        <v>221</v>
+      </c>
+      <c r="D167" t="s">
+        <v>81</v>
+      </c>
+      <c r="E167" t="s">
+        <v>117</v>
+      </c>
+      <c r="F167" s="1"/>
+    </row>
+    <row r="168" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>124</v>
+      </c>
+      <c r="C168" t="s">
+        <v>222</v>
+      </c>
+      <c r="D168" t="s">
+        <v>81</v>
+      </c>
+      <c r="E168" t="s">
+        <v>117</v>
+      </c>
+      <c r="F168" s="1"/>
+    </row>
+    <row r="169" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>125</v>
+      </c>
+      <c r="C169" t="s">
+        <v>223</v>
+      </c>
+      <c r="F169" s="1"/>
+    </row>
+    <row r="170" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>126</v>
+      </c>
+      <c r="C170" t="s">
+        <v>224</v>
+      </c>
+      <c r="F170" s="1"/>
+    </row>
+    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F171" s="1"/>
+    </row>
+    <row r="172" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F172" s="1"/>
+    </row>
+    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F173" s="1"/>
+    </row>
+    <row r="174" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F174" s="1"/>
+    </row>
+    <row r="175" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F175" s="1"/>
+    </row>
+    <row r="176" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F176" s="1"/>
+    </row>
+    <row r="177" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F177" s="1"/>
+    </row>
+    <row r="178" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F178" s="1"/>
+    </row>
+    <row r="179" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F179" s="1"/>
+    </row>
+    <row r="180" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F180" s="1"/>
+    </row>
+    <row r="181" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F181" s="1"/>
+    </row>
+    <row r="182" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F182" s="1"/>
+    </row>
+    <row r="183" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F183" s="1"/>
+    </row>
+    <row r="184" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F184" s="1"/>
+    </row>
+    <row r="185" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F185" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor updates made to USB documentation and FMEA.
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="234">
   <si>
     <t>Rocket Tracks FMEA Analysis</t>
   </si>
@@ -715,6 +715,12 @@
   </si>
   <si>
     <t>PFBOUT, PFBIN1, PFBIN2 grounded</t>
+  </si>
+  <si>
+    <t>fail output high or fail output low</t>
+  </si>
+  <si>
+    <t>no data being sent via ethernet</t>
   </si>
 </sst>
 </file>
@@ -892,9 +898,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1084,6 +1087,9 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1121,63 +1127,63 @@
     <tableColumn id="2" name="Item" dataDxfId="31"/>
     <tableColumn id="3" name="Potential failure mode" dataDxfId="30"/>
     <tableColumn id="4" name="Potential cause(s)" dataDxfId="29"/>
-    <tableColumn id="6" name="local effects of failure" dataDxfId="0"/>
-    <tableColumn id="7" name="next higher level effect" dataDxfId="28"/>
-    <tableColumn id="8" name="system level end effect" dataDxfId="27"/>
-    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="26"/>
-    <tableColumn id="10" name="(S) Severity" dataDxfId="25"/>
-    <tableColumn id="12" name="Risk Level" dataDxfId="24"/>
-    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="23"/>
-    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="22"/>
+    <tableColumn id="6" name="local effects of failure" dataDxfId="28"/>
+    <tableColumn id="7" name="next higher level effect" dataDxfId="27"/>
+    <tableColumn id="8" name="system level end effect" dataDxfId="26"/>
+    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="25"/>
+    <tableColumn id="10" name="(S) Severity" dataDxfId="24"/>
+    <tableColumn id="12" name="Risk Level" dataDxfId="23"/>
+    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="22"/>
+    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B4:C9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="19"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="18"/>
+    <tableColumn id="1" name="Rating" dataDxfId="18"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="B13:C19"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="15"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="14"/>
+    <tableColumn id="1" name="Rating" dataDxfId="14"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="B23:C29"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="11"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="10"/>
+    <tableColumn id="1" name="Rating" dataDxfId="10"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="G4:M9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Probability \ Severity" dataDxfId="7"/>
-    <tableColumn id="2" name="I" dataDxfId="6"/>
-    <tableColumn id="3" name="II" dataDxfId="5"/>
-    <tableColumn id="4" name="III" dataDxfId="4"/>
-    <tableColumn id="5" name="IV" dataDxfId="3"/>
-    <tableColumn id="6" name="V" dataDxfId="2"/>
-    <tableColumn id="7" name="VI" dataDxfId="1"/>
+    <tableColumn id="1" name="Probability \ Severity" dataDxfId="6"/>
+    <tableColumn id="2" name="I" dataDxfId="5"/>
+    <tableColumn id="3" name="II" dataDxfId="4"/>
+    <tableColumn id="4" name="III" dataDxfId="3"/>
+    <tableColumn id="5" name="IV" dataDxfId="2"/>
+    <tableColumn id="6" name="V" dataDxfId="1"/>
+    <tableColumn id="7" name="VI" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1472,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,6 +3285,9 @@
       <c r="C75" t="s">
         <v>146</v>
       </c>
+      <c r="D75" t="s">
+        <v>232</v>
+      </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
@@ -3717,6 +3726,9 @@
       <c r="F108" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="G108" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="109" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B109">
@@ -3734,6 +3746,9 @@
       <c r="F109" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="G109" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="110" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B110">
@@ -3751,6 +3766,9 @@
       <c r="F110" s="1" t="s">
         <v>229</v>
       </c>
+      <c r="G110" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="111" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B111">
@@ -3767,6 +3785,9 @@
       </c>
       <c r="F111" s="1" t="s">
         <v>230</v>
+      </c>
+      <c r="G111" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated layout of Rtx Controller Board.
</commit_message>
<xml_diff>
--- a/Documentation/FMEA/fmea.xlsx
+++ b/Documentation/FMEA/fmea.xlsx
@@ -2257,7 +2257,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="156">
     <dxf>
       <font>
         <b/>
@@ -2325,6 +2325,218 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2721,43 +2933,50 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2766,170 +2985,17 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -2945,178 +3011,211 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table112" displayName="Table112" ref="B7:N24" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table112" displayName="Table112" ref="B7:N24" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
   <autoFilter ref="B7:N24"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="102"/>
-    <tableColumn id="2" name="Item" dataDxfId="101"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="100"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="99"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="98"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="97"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="96"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="95"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="94"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="93"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="92"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="91"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="90"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="153"/>
+    <tableColumn id="2" name="Item" dataDxfId="152"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="151"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="150"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="149"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="148"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="147"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="146"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="145"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="144"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="143"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="142"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
-  <autoFilter ref="B13:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="B4:C9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="119"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="118"/>
+    <tableColumn id="1" name="Rating" dataDxfId="33"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
-  <autoFilter ref="B23:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B13:C19" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="B13:C19"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="115"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="114"/>
+    <tableColumn id="1" name="Rating" dataDxfId="29"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B23:C29" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B23:C29"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Rating" dataDxfId="25"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="G4:M9" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="G4:M9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Probability \ Severity" dataDxfId="111"/>
-    <tableColumn id="2" name="I" dataDxfId="110"/>
-    <tableColumn id="3" name="II" dataDxfId="109"/>
-    <tableColumn id="4" name="III" dataDxfId="108"/>
-    <tableColumn id="5" name="IV" dataDxfId="107"/>
-    <tableColumn id="6" name="V" dataDxfId="106"/>
-    <tableColumn id="7" name="VI" dataDxfId="105"/>
+    <tableColumn id="1" name="Probability \ Severity" dataDxfId="21"/>
+    <tableColumn id="2" name="I" dataDxfId="20"/>
+    <tableColumn id="3" name="II" dataDxfId="19"/>
+    <tableColumn id="4" name="III" dataDxfId="18"/>
+    <tableColumn id="5" name="IV" dataDxfId="17"/>
+    <tableColumn id="6" name="V" dataDxfId="16"/>
+    <tableColumn id="7" name="VI" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table415" displayName="Table415" ref="B28:N60" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table415" displayName="Table415" ref="B28:N60" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
   <autoFilter ref="B28:N60"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="87"/>
-    <tableColumn id="2" name="Item" dataDxfId="86"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="85"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="84"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="83"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="82"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="81"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="80"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="79"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="78"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="77"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="76"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="75"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="138"/>
+    <tableColumn id="2" name="Item" dataDxfId="137"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="136"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="135"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="134"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="133"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="132"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="131"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="130"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="129"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="128"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="127"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table916" displayName="Table916" ref="B141:N170" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table916" displayName="Table916" ref="B141:N170" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="B141:N170"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="72"/>
-    <tableColumn id="2" name="Item" dataDxfId="71"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="70"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="69"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="68"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="67"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="66"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="65"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="64"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="63"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="62"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="61"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="60"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="123"/>
+    <tableColumn id="2" name="Item" dataDxfId="122"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="121"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="120"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="119"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="118"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="117"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="116"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="115"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="114"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="113"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="112"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1017" displayName="Table1017" ref="B173:N182" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1017" displayName="Table1017" ref="B173:N182" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
   <autoFilter ref="B173:N182"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="57"/>
-    <tableColumn id="2" name="Item" dataDxfId="56"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="55"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="54"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="53"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="52"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="51"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="50"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="49"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="48"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="47"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="46"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="45"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="108"/>
+    <tableColumn id="2" name="Item" dataDxfId="107"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="106"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="105"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="104"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="103"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="102"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="101"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="100"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="99"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="98"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="97"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1218" displayName="Table1218" ref="B185:N203" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1218" displayName="Table1218" ref="B185:N203" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="B185:N203"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="42"/>
-    <tableColumn id="2" name="Item" dataDxfId="41"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="40"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="39"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="38"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="37"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="36"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="35"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="34"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="33"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="32"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="31"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="30"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="93"/>
+    <tableColumn id="2" name="Item" dataDxfId="92"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="91"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="90"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="89"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="88"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="87"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="86"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="85"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="84"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="83"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="82"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1319" displayName="Table1319" ref="B207:N213" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1319" displayName="Table1319" ref="B207:N213" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="B207:N213"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="27"/>
-    <tableColumn id="2" name="Item" dataDxfId="26"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="25"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="24"/>
-    <tableColumn id="5" name="local effects of failure" dataDxfId="23"/>
-    <tableColumn id="6" name="next higher level effect" dataDxfId="22"/>
-    <tableColumn id="7" name="system level end effect" dataDxfId="21"/>
-    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="20"/>
-    <tableColumn id="9" name="(S) Severity" dataDxfId="19"/>
-    <tableColumn id="10" name="Risk Level" dataDxfId="18"/>
-    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="17"/>
-    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="16"/>
-    <tableColumn id="13" name="Fix in FW" dataDxfId="15"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="78"/>
+    <tableColumn id="2" name="Item" dataDxfId="77"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="76"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="75"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="74"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="73"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="72"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="71"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="70"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="69"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="68"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="67"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="B64:N135" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="B64:N135" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="B64:N135"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="63"/>
+    <tableColumn id="2" name="Item" dataDxfId="62"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="61"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="60"/>
+    <tableColumn id="5" name="local effects of failure" dataDxfId="59"/>
+    <tableColumn id="6" name="next higher level effect" dataDxfId="58"/>
+    <tableColumn id="7" name="system level end effect" dataDxfId="57"/>
+    <tableColumn id="8" name="(P) Probability (estimate)" dataDxfId="56"/>
+    <tableColumn id="9" name="(S) Severity" dataDxfId="55"/>
+    <tableColumn id="10" name="Risk Level" dataDxfId="54"/>
+    <tableColumn id="11" name="Actions for further Investigation" dataDxfId="53"/>
+    <tableColumn id="12" name="Mitigation / Requirements" dataDxfId="52"/>
+    <tableColumn id="13" name="Fix in FW" dataDxfId="51"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B217:N246" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B217:N246"/>
   <tableColumns count="13">
     <tableColumn id="1" name="FMEA Ref. #" dataDxfId="14"/>
     <tableColumn id="2" name="Item" dataDxfId="13"/>
@@ -3136,36 +3235,25 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B5:N41" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B5:N41" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="B5:N41"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="138"/>
-    <tableColumn id="2" name="Item" dataDxfId="137"/>
-    <tableColumn id="3" name="Potential failure mode" dataDxfId="136"/>
-    <tableColumn id="4" name="Potential cause(s)" dataDxfId="135"/>
-    <tableColumn id="6" name="local effects of failure" dataDxfId="134"/>
-    <tableColumn id="7" name="next higher level effect" dataDxfId="133"/>
-    <tableColumn id="8" name="system level end effect" dataDxfId="132"/>
-    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="131"/>
-    <tableColumn id="10" name="(S) Severity" dataDxfId="130"/>
-    <tableColumn id="12" name="Risk Level" dataDxfId="129"/>
-    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="128"/>
-    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="127"/>
-    <tableColumn id="5" name="Fix in FW" dataDxfId="126"/>
+    <tableColumn id="1" name="FMEA Ref. #" dataDxfId="48"/>
+    <tableColumn id="2" name="Item" dataDxfId="47"/>
+    <tableColumn id="3" name="Potential failure mode" dataDxfId="46"/>
+    <tableColumn id="4" name="Potential cause(s)" dataDxfId="45"/>
+    <tableColumn id="6" name="local effects of failure" dataDxfId="44"/>
+    <tableColumn id="7" name="next higher level effect" dataDxfId="43"/>
+    <tableColumn id="8" name="system level end effect" dataDxfId="42"/>
+    <tableColumn id="9" name="(P) Probability (estimate)" dataDxfId="41"/>
+    <tableColumn id="10" name="(S) Severity" dataDxfId="40"/>
+    <tableColumn id="12" name="Risk Level" dataDxfId="39"/>
+    <tableColumn id="13" name="Actions for further Investigation" dataDxfId="38"/>
+    <tableColumn id="14" name="Mitigation / Requirements" dataDxfId="37"/>
+    <tableColumn id="5" name="Fix in FW" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:C9" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
-  <autoFilter ref="B4:C9"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Rating" dataDxfId="123"/>
-    <tableColumn id="2" name="Meaning" dataDxfId="122"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3458,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8443,7 +8531,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="7">
+  <tableParts count="8">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -8451,6 +8539,7 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>